<commit_message>
Pre and Post tests added
</commit_message>
<xml_diff>
--- a/I_Pause Menu Help.xlsx
+++ b/I_Pause Menu Help.xlsx
@@ -5,6 +5,8 @@
   <sheets>
     <sheet state="visible" name="Stories" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Test I01" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Pre - Test" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Post - Test" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +14,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="34">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>User Stories</t>
+  </si>
+  <si>
+    <t>As an expert gamer, I would like access to have the help menu on the pause screen so that I can learn about the various enemies and how they will attack me.</t>
+  </si>
   <si>
     <t>Test ID</t>
   </si>
@@ -20,7 +34,7 @@
     <t>I01</t>
   </si>
   <si>
-    <t>ID</t>
+    <t>As a novice gamer, I would access to the help menu on the pause screen so I can learn how to play the game.</t>
   </si>
   <si>
     <t>Test Owner</t>
@@ -29,6 +43,15 @@
     <t>Victoria Gorski</t>
   </si>
   <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>JW</t>
+  </si>
+  <si>
+    <t>Approval</t>
+  </si>
+  <si>
     <t>Dependancies</t>
   </si>
   <si>
@@ -68,6 +91,9 @@
     <t xml:space="preserve">game loads </t>
   </si>
   <si>
+    <t>P</t>
+  </si>
+  <si>
     <t xml:space="preserve">Select either the Wave mode or Easy Mode </t>
   </si>
   <si>
@@ -83,28 +109,13 @@
     <t xml:space="preserve">Select the Help Menu option </t>
   </si>
   <si>
+    <t>User will be able to press the help menu key and access the help menu</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
     <t xml:space="preserve">User will be able to press the help menu key but will not have access to said menu </t>
-  </si>
-  <si>
-    <t>Approval</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>User Stories</t>
-  </si>
-  <si>
-    <t>As an expert gamer, I would like access to have the help menu on the pause screen so that I can learn about the various enemies and how they will attack me.</t>
-  </si>
-  <si>
-    <t>As a novice gamer, I would access to the help menu on the pause screen so I can learn how to play the game.</t>
-  </si>
-  <si>
-    <t>TC</t>
-  </si>
-  <si>
-    <t>JW</t>
   </si>
 </sst>
 </file>
@@ -119,14 +130,21 @@
     </font>
     <font>
       <b/>
+    </font>
+    <font/>
+    <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <b/>
       <name val="Arial"/>
@@ -134,15 +152,8 @@
     <font>
       <name val="Arial"/>
     </font>
-    <font>
-      <b/>
-    </font>
-    <font>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,18 +162,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border/>
     <border>
       <left style="thin">
@@ -208,6 +213,17 @@
       </bottom>
     </border>
     <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -233,80 +249,112 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -320,6 +368,14 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -528,51 +584,51 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>30</v>
+      <c r="A3" s="12"/>
+      <c r="B3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>29</v>
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="28"/>
+      <c r="A5" s="19"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -590,141 +646,151 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="43.43"/>
+    <col customWidth="1" min="3" max="3" width="34.43"/>
+    <col customWidth="1" min="4" max="4" width="7.43"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
+      <c r="A2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
+      <c r="A3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
+      <c r="A4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
+      <c r="A5" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
+      <c r="A6" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="30">
+        <v>2.0</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="30">
+        <v>3.0</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="30">
+        <v>4.0</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="19"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="19"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="19"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="16">
-        <v>4.0</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="19"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -739,4 +805,342 @@
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="29">
+        <v>2.0</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="29">
+        <v>3.0</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="29">
+        <v>4.0</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B13:D13"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="29">
+        <v>1.0</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="29">
+        <v>2.0</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="29">
+        <v>3.0</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="29">
+        <v>4.0</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B13:D13"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>